<commit_message>
delete all .pkl files and convert all dataframes to .xlsx
</commit_message>
<xml_diff>
--- a/dataframe_each_make_xlsx_file/df_ford_new.xlsx
+++ b/dataframe_each_make_xlsx_file/df_ford_new.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G291"/>
+  <dimension ref="A1:G292"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9964,7 +9964,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Focus (Push To Start)</t>
+          <t>Focus (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -9997,7 +9997,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Taurus (Keyed Ignition)</t>
+          <t>Focus (Push To Start)</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -10030,20 +10030,53 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
+          <t>Taurus (Keyed Ignition)</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>Parameter Reset Required</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>PATS Type C</t>
+        </is>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>Instrument Cluster</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="n">
+        <v>290</v>
+      </c>
+      <c r="B292" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
           <t>Taurus (Push To Start)</t>
         </is>
       </c>
-      <c r="E291" t="inlineStr">
-        <is>
-          <t>Parameter Reset Required</t>
-        </is>
-      </c>
-      <c r="F291" t="inlineStr">
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>Parameter Reset Required</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
         <is>
           <t>PATS Type C</t>
         </is>
       </c>
-      <c r="G291" t="inlineStr">
+      <c r="G292" t="inlineStr">
         <is>
           <t>Instrument Cluster</t>
         </is>

</xml_diff>